<commit_message>
Updated Dataset Key.xlsx and .gitignore
</commit_message>
<xml_diff>
--- a/Dataset Key.xlsx
+++ b/Dataset Key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlima/Documents/GitHub/reconfigurable-solar-cells/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F875741-A72E-E34E-84F6-36393EB834DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F0811A-3FF6-E44B-8E4C-B0D68E88F356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{D03FEAF9-A323-DD42-AAE4-45997B47A029}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Shading Map Code</t>
   </si>
@@ -87,14 +87,43 @@
   </si>
   <si>
     <t>First column at 3, rest at 7</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>TCT</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>MPP</t>
+  </si>
+  <si>
+    <t>C02P5</t>
+  </si>
+  <si>
+    <t>S04P5</t>
+  </si>
+  <si>
+    <t>S05P5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -143,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -151,6 +180,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,6 +462,359 @@
         <a:xfrm>
           <a:off x="2260600" y="15176500"/>
           <a:ext cx="2763236" cy="1435100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1003299</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3962500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2159000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{553BB4EB-9EEA-9A46-A41B-4C1D5EB17D2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7823199" y="3035300"/>
+          <a:ext cx="2959201" cy="1993900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>927100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3594100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1930400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDAB65DF-0F74-7848-A4E7-12238BE8BBE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7747000" y="5270500"/>
+          <a:ext cx="2667000" cy="1778000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>927100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>495300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3956050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2514600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{180BA50D-5163-D942-AFD1-00FB5DC02261}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7747000" y="15100300"/>
+          <a:ext cx="3028950" cy="2019300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4191000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2599267</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69946041-B181-D043-8A61-0EA14194F190}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7378700" y="17843500"/>
+          <a:ext cx="3632200" cy="2421467"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>110435</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>834950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2981739</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2280110</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAB0A73F-CC58-364F-9491-AF1FE31C0B3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1969421" y="21339008"/>
+          <a:ext cx="2871304" cy="1445160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>182965</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1022459</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3102352</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2529239</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3295C72B-06AA-6946-9481-BDEB95B77673}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2044914" y="24366781"/>
+          <a:ext cx="2919387" cy="1506780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>473559</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>182966</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4313263</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2742769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1C9B9BB-E94F-FF4D-8FC1-A8206F889315}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7286356" y="23527288"/>
+          <a:ext cx="3839704" cy="2559803"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>204492</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>269068</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3093997</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1765086</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A440C986-A6E7-F94A-AA47-79D5614ACA64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2066441" y="26519322"/>
+          <a:ext cx="2889505" cy="1496018"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -740,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5A1329-3D34-824E-9BD6-BFD7C34C5F99}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -752,27 +1135,39 @@
     <col min="2" max="2" width="44.5" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="60.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+    <col min="5" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -786,8 +1181,11 @@
       <c r="E2" s="1">
         <v>64000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="1">
+        <v>202.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -801,20 +1199,26 @@
       <c r="E3" s="1">
         <v>125000</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="str">
+      <c r="F3" s="1">
+        <v>229.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="str">
         <f>_xlfn.CONCAT(A4,".xslx")</f>
         <v>﻿R01P5.xslx</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>64000</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="170" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="1">
+        <v>184.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="170" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -822,7 +1226,7 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="166" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="166" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -830,14 +1234,17 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="str">
-        <f>_xlfn.CONCAT(A6,".xslx")</f>
+        <f t="shared" ref="C6:C12" si="0">_xlfn.CONCAT(A6,".xslx")</f>
         <v>S01P5.xslx</v>
       </c>
       <c r="E6" s="1">
         <v>64000</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -845,35 +1252,80 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="str">
-        <f>_xlfn.CONCAT(A7,".xslx")</f>
+        <f t="shared" si="0"/>
         <v>S02P5.xslx</v>
       </c>
       <c r="E7" s="1">
         <v>64000</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="F7" s="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4" t="str">
-        <f>_xlfn.CONCAT(A8,".xslx")</f>
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>S03P5.xslx</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>64000</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" ht="224" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="F8" s="1">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="224" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4" t="str">
-        <f>_xlfn.CONCAT(A9,".xslx")</f>
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>C01P5.xslx</v>
+      </c>
+      <c r="E9" s="1">
+        <v>64000</v>
+      </c>
+      <c r="F9" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="223" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>C02P5.xslx</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="229" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S04P5.xslx</v>
+      </c>
+      <c r="E11" s="1">
+        <v>64000</v>
+      </c>
+      <c r="F11" s="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="157" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>S05P5.xslx</v>
       </c>
     </row>
   </sheetData>
@@ -884,7 +1336,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC721700-1AB0-104E-99BB-9F6A073030E6}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="A1:F10"/>
@@ -894,39 +1346,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3">
-        <v>2.5</v>
+        <v>9.5</v>
       </c>
       <c r="B1" s="3">
-        <v>2.5</v>
+        <v>9.5</v>
       </c>
       <c r="C1" s="3">
-        <v>2.5</v>
+        <v>9.5</v>
       </c>
       <c r="D1" s="3">
-        <v>2.5</v>
+        <v>8.5</v>
       </c>
       <c r="E1" s="3">
-        <v>2.5</v>
+        <v>7</v>
       </c>
       <c r="F1" s="3">
-        <v>2.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
-        <v>5</v>
+        <v>9.5</v>
       </c>
       <c r="B2" s="3">
-        <v>2.5</v>
+        <v>9.5</v>
       </c>
       <c r="C2" s="3">
-        <v>2.5</v>
+        <v>9.5</v>
       </c>
       <c r="D2" s="3">
-        <v>2.5</v>
+        <v>8.5</v>
       </c>
       <c r="E2" s="3">
-        <v>2.5</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3">
         <v>5</v>
@@ -934,19 +1386,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="E3" s="3">
         <v>5</v>
-      </c>
-      <c r="B3" s="3">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3">
-        <v>7</v>
       </c>
       <c r="F3" s="3">
         <v>5</v>
@@ -954,19 +1406,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="B4" s="3">
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="C4" s="3">
         <v>8.5</v>
       </c>
       <c r="D4" s="3">
-        <v>8.5</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3">
         <v>5</v>
@@ -974,19 +1426,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3">
         <v>5</v>
-      </c>
-      <c r="B5" s="3">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3">
-        <v>9.5</v>
-      </c>
-      <c r="D5" s="3">
-        <v>9.5</v>
-      </c>
-      <c r="E5" s="3">
-        <v>7</v>
       </c>
       <c r="F5" s="3">
         <v>5</v>
@@ -994,19 +1446,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3">
-        <v>9.5</v>
-      </c>
-      <c r="D6" s="3">
-        <v>9.5</v>
-      </c>
       <c r="E6" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3">
         <v>5</v>
@@ -1014,19 +1466,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3">
-        <v>8.5</v>
-      </c>
       <c r="D7" s="3">
-        <v>8.5</v>
+        <v>5</v>
       </c>
       <c r="E7" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F7" s="3">
         <v>5</v>
@@ -1034,62 +1486,262 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D8" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E8" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F8" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="E9" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F9" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D10" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E10" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F10" s="3">
-        <v>2.5</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3">
+        <v>3</v>
+      </c>
+      <c r="F15" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3</v>
+      </c>
+      <c r="F16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3">
+        <v>7</v>
+      </c>
+      <c r="F18" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3">
+        <v>7</v>
+      </c>
+      <c r="E19" s="3">
+        <v>7</v>
+      </c>
+      <c r="F19" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3">
+        <v>7</v>
+      </c>
+      <c r="D20" s="3">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3">
+        <v>7</v>
+      </c>
+      <c r="F20" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3">
+        <v>7</v>
+      </c>
+      <c r="E21" s="3">
+        <v>7</v>
+      </c>
+      <c r="F21" s="3">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
C02, S04, S05 datasets created
</commit_message>
<xml_diff>
--- a/Dataset Key.xlsx
+++ b/Dataset Key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlima/Documents/GitHub/reconfigurable-solar-cells/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F0811A-3FF6-E44B-8E4C-B0D68E88F356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E708F2-3A9A-2A4C-A187-D19DA4822D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{D03FEAF9-A323-DD42-AAE4-45997B47A029}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Shading Map Code</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>S05P5</t>
+  </si>
+  <si>
+    <t>S05P10</t>
+  </si>
+  <si>
+    <t>S05P2</t>
   </si>
 </sst>
 </file>
@@ -175,12 +181,12 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -253,15 +259,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>828040</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2123440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3962400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>3952240</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2085340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -284,8 +290,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7658100" y="7327900"/>
-          <a:ext cx="3124200" cy="2082800"/>
+          <a:off x="7655560" y="9408160"/>
+          <a:ext cx="3124200" cy="2087880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -299,13 +305,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>698500</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>347980</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>4267200</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2544233</xdr:rowOff>
+      <xdr:rowOff>2727113</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -328,7 +334,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6921500" y="9232900"/>
+          <a:off x="7526020" y="11910060"/>
           <a:ext cx="3568700" cy="2379133"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -340,13 +346,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>139700</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>3035300</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>1794498</xdr:rowOff>
@@ -384,13 +390,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>3086100</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1756398</xdr:rowOff>
@@ -428,13 +434,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>393700</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>571500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>3156936</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>2006600</xdr:rowOff>
@@ -519,13 +525,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>927100</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3594100</xdr:colOff>
+      <xdr:colOff>3797300</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1930400</xdr:rowOff>
+      <xdr:rowOff>2065866</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -548,8 +554,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7747000" y="5270500"/>
-          <a:ext cx="2667000" cy="1778000"/>
+          <a:off x="7747000" y="5270499"/>
+          <a:ext cx="2870200" cy="1913467"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -648,13 +654,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>110435</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>834950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>2981739</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>2280110</xdr:rowOff>
@@ -693,13 +699,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>182965</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>1022459</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>3102352</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>2529239</xdr:rowOff>
@@ -744,9 +750,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4313263</xdr:colOff>
+      <xdr:colOff>2565400</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>2742769</xdr:rowOff>
+      <xdr:rowOff>1577527</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -769,8 +775,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7286356" y="23527288"/>
-          <a:ext cx="3839704" cy="2559803"/>
+          <a:off x="7293459" y="23322366"/>
+          <a:ext cx="2091841" cy="1394561"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -781,15 +787,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>204492</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>269068</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>3093997</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>1765086</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -815,6 +821,314 @@
         <a:xfrm>
           <a:off x="2066441" y="26519322"/>
           <a:ext cx="2889505" cy="1496018"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1016000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2478893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3893736</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1898023</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC9D9641-BF90-DB4D-B017-97715F9B3301}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7843520" y="28539293"/>
+          <a:ext cx="2877736" cy="1918490"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>781538</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>93039</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4244313</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>2401556</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD2CE9F5-A5CD-4542-9D7E-E9A72CD9149E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7606043" y="28340072"/>
+          <a:ext cx="3462775" cy="2308517"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>844343</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>111648</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4256595</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2386482</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67585380-A3D0-674E-B27E-EA4244167097}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7668848" y="26362967"/>
+          <a:ext cx="3412252" cy="2274834"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314960</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>20320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4439920</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2770293</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACA67DE1-B774-0B40-A95A-655C7CD69A66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7142480" y="20340320"/>
+          <a:ext cx="4124960" cy="2749973"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3133345</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1953218</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75EC5380-C8DF-3C46-A45D-2288EFE90396}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3677920" y="26517600"/>
+          <a:ext cx="2889505" cy="1496018"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>538480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3092705</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>2034498</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B3BD2D0-E9C4-8644-AC6D-C46366C0DFA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3637280" y="31089600"/>
+          <a:ext cx="2889505" cy="1496018"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2565400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1562100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4394200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2781300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6E12212-DE4B-D342-B2C7-E1783DCD0733}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9385300" y="24701500"/>
+          <a:ext cx="1828800" cy="1219200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1123,17 +1437,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5A1329-3D34-824E-9BD6-BFD7C34C5F99}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="180" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="44.5" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
     <col min="4" max="4" width="60.33203125" customWidth="1"/>
     <col min="5" max="6" width="21" customWidth="1"/>
   </cols>
@@ -1143,19 +1458,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>19</v>
@@ -1168,165 +1483,265 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="str">
+      <c r="B2" s="3" t="str">
         <f>_xlfn.CONCAT(A2,".xslx")</f>
         <v>B9378P5.xslx</v>
       </c>
-      <c r="E2" s="1">
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>202.3</v>
+      </c>
+      <c r="F2" s="3">
         <v>64000</v>
       </c>
-      <c r="F2" s="1">
-        <v>202.3</v>
-      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="str">
+      <c r="B3" s="3" t="str">
         <f>_xlfn.CONCAT(A3,".xslx")</f>
         <v>B9378P10.xslx</v>
       </c>
-      <c r="E3" s="1">
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>229.7</v>
+      </c>
+      <c r="F3" s="3">
         <v>125000</v>
       </c>
-      <c r="F3" s="1">
-        <v>229.7</v>
-      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="str">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="str">
         <f>_xlfn.CONCAT(A4,".xslx")</f>
         <v>﻿R01P5.xslx</v>
       </c>
-      <c r="E4" s="1">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>184.8</v>
+      </c>
+      <c r="F4" s="3">
         <v>64000</v>
       </c>
-      <c r="F4" s="1">
-        <v>184.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="154" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
         <v>64000</v>
       </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="166" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="str">
+        <f>_xlfn.CONCAT(A6,".xslx")</f>
+        <v>S01P5.xslx</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="str">
-        <f t="shared" ref="C6:C12" si="0">_xlfn.CONCAT(A6,".xslx")</f>
-        <v>S01P5.xslx</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>230</v>
+      </c>
+      <c r="F6" s="3">
         <v>64000</v>
       </c>
-      <c r="F6" s="1">
-        <v>230</v>
-      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="str">
+        <f>_xlfn.CONCAT(A7,".xslx")</f>
+        <v>S02P5.xslx</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>S02P5.xslx</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
+        <v>202</v>
+      </c>
+      <c r="F7" s="3">
         <v>64000</v>
       </c>
-      <c r="F7" s="1">
-        <v>202</v>
-      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="str">
+        <f>_xlfn.CONCAT(A8,".xslx")</f>
+        <v>S03P5.xslx</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>S03P5.xslx</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>219</v>
+      </c>
+      <c r="F8" s="3">
         <v>64000</v>
       </c>
-      <c r="F8" s="1">
-        <v>219</v>
-      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" ht="224" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="B9" s="3" t="str">
+        <f>_xlfn.CONCAT(A9,".xslx")</f>
         <v>C01P5.xslx</v>
       </c>
-      <c r="E9" s="1">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
+        <v>146</v>
+      </c>
+      <c r="F9" s="3">
         <v>64000</v>
       </c>
-      <c r="F9" s="1">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="223" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" ht="223" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="B10" s="3" t="str">
+        <f>_xlfn.CONCAT(A10,".xslx")</f>
         <v>C02P5.xslx</v>
       </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="229" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="B11" s="3" t="str">
+        <f>_xlfn.CONCAT(A11,".xslx")</f>
         <v>S04P5.xslx</v>
       </c>
-      <c r="E11" s="1">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
+        <v>170</v>
+      </c>
+      <c r="F11" s="3">
         <v>64000</v>
       </c>
-      <c r="F11" s="1">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" ht="157" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3" t="str">
+        <f>_xlfn.CONCAT(A12,".xslx")</f>
+        <v>S05P2.xslx</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>225</v>
+      </c>
+      <c r="F12" s="3">
+        <v>64000</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="157" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="B13" s="3" t="str">
+        <f>_xlfn.CONCAT(A13,".xslx")</f>
         <v>S05P5.xslx</v>
       </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
+        <v>209</v>
+      </c>
+      <c r="F13" s="3">
+        <v>64000</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="196" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="3" t="str">
+        <f>_xlfn.CONCAT(A14,".xslx")</f>
+        <v>S05P10.xslx</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
+        <v>192</v>
+      </c>
+      <c r="F14" s="3">
+        <v>64000</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1339,408 +1754,408 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="A1:F10"/>
+      <selection activeCell="A12" sqref="A12:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="3">
+      <c r="A1" s="2">
         <v>9.5</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="2">
         <v>9.5</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="2">
         <v>9.5</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="2">
         <v>8.5</v>
       </c>
-      <c r="E1" s="3">
-        <v>7</v>
-      </c>
-      <c r="F1" s="3">
+      <c r="E1" s="2">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>9.5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>9.5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>9.5</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>8.5</v>
       </c>
-      <c r="E2" s="3">
-        <v>7</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2" s="2">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>9.5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>9.5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>9.5</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>8.5</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>5</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>8.5</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>8.5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>8.5</v>
       </c>
-      <c r="D4" s="3">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="D4" s="2">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2">
         <v>5</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>8.5</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>8.5</v>
       </c>
-      <c r="C5" s="3">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3">
-        <v>7</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="C5" s="2">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2">
         <v>5</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="A6" s="2">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2">
         <v>5</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>5</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="A7" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2">
         <v>5</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>5</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>5</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>4</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>4</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>4</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="3">
-        <v>3</v>
-      </c>
-      <c r="C9" s="3">
-        <v>3</v>
-      </c>
-      <c r="D9" s="3">
-        <v>3</v>
-      </c>
-      <c r="E9" s="3">
-        <v>3</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3">
-        <v>3</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="A10" s="2">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
         <v>2</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>2</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>2</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3">
-        <v>7</v>
-      </c>
-      <c r="C12" s="3">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3">
-        <v>7</v>
-      </c>
-      <c r="E12" s="3">
-        <v>7</v>
-      </c>
-      <c r="F12" s="3">
+      <c r="A12" s="2">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3">
-        <v>7</v>
-      </c>
-      <c r="E13" s="3">
-        <v>3</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="A13" s="2">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3">
-        <v>7</v>
-      </c>
-      <c r="C14" s="3">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3">
-        <v>3</v>
-      </c>
-      <c r="E14" s="3">
-        <v>3</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="A14" s="2">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3">
-        <v>7</v>
-      </c>
-      <c r="C15" s="3">
-        <v>3</v>
-      </c>
-      <c r="D15" s="3">
-        <v>3</v>
-      </c>
-      <c r="E15" s="3">
-        <v>3</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="A15" s="2">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3">
-        <v>3</v>
-      </c>
-      <c r="D16" s="3">
-        <v>3</v>
-      </c>
-      <c r="E16" s="3">
-        <v>3</v>
-      </c>
-      <c r="F16" s="3">
+      <c r="A16" s="2">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>3</v>
-      </c>
-      <c r="B17" s="3">
-        <v>3</v>
-      </c>
-      <c r="C17" s="3">
-        <v>3</v>
-      </c>
-      <c r="D17" s="3">
-        <v>3</v>
-      </c>
-      <c r="E17" s="3">
-        <v>3</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3">
-        <v>3</v>
-      </c>
-      <c r="C18" s="3">
-        <v>3</v>
-      </c>
-      <c r="D18" s="3">
-        <v>3</v>
-      </c>
-      <c r="E18" s="3">
-        <v>7</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="A18" s="2">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>3</v>
-      </c>
-      <c r="B19" s="3">
-        <v>3</v>
-      </c>
-      <c r="C19" s="3">
-        <v>3</v>
-      </c>
-      <c r="D19" s="3">
-        <v>7</v>
-      </c>
-      <c r="E19" s="3">
-        <v>7</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="A19" s="2">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+      <c r="D19" s="2">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2">
+        <v>7</v>
+      </c>
+      <c r="F19" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>3</v>
-      </c>
-      <c r="B20" s="3">
-        <v>3</v>
-      </c>
-      <c r="C20" s="3">
-        <v>7</v>
-      </c>
-      <c r="D20" s="3">
-        <v>7</v>
-      </c>
-      <c r="E20" s="3">
-        <v>7</v>
-      </c>
-      <c r="F20" s="3">
+      <c r="A20" s="2">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <v>3</v>
-      </c>
-      <c r="B21" s="3">
-        <v>7</v>
-      </c>
-      <c r="C21" s="3">
-        <v>7</v>
-      </c>
-      <c r="D21" s="3">
-        <v>7</v>
-      </c>
-      <c r="E21" s="3">
-        <v>7</v>
-      </c>
-      <c r="F21" s="3">
+      <c r="A21" s="2">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2">
+        <v>7</v>
+      </c>
+      <c r="D21" s="2">
+        <v>7</v>
+      </c>
+      <c r="E21" s="2">
+        <v>7</v>
+      </c>
+      <c r="F21" s="2">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Re-running R01P5 and S03P5
As well as running R01P10.
</commit_message>
<xml_diff>
--- a/Dataset Key.xlsx
+++ b/Dataset Key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlima/Documents/GitHub/reconfigurable-solar-cells/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E708F2-3A9A-2A4C-A187-D19DA4822D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E711618F-B3BF-9E4E-A9CD-95A702DEEC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{D03FEAF9-A323-DD42-AAE4-45997B47A029}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Shading Map Code</t>
   </si>
@@ -115,12 +115,18 @@
   <si>
     <t>S05P2</t>
   </si>
+  <si>
+    <t>8.395496 0.424943 0.854863 8.844951 0.522385 8.320303 6.383254 8.454816 0.659086 8.689136 0.2 8.68987 8.847101 0.853958 @.993618 8.733088 0.659951 0.67742 0.393654 0.2 0.621482 6.573741 - 0.2 0.548724 @.674576 8.683729 8.498921 0.2 1 8.339769 - 0.2 0.938431 0.2 6.554465 6.913284 8.488619 0.891248 8.511976 8.388388 .569149 0.572895 0.2 0.656584 0.676249 0.61884 0.632691 0.63422 6.763861 8.716159 6.353372 0.600189</t>
+  </si>
+  <si>
+    <t>C03P5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,6 +138,19 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -174,11 +193,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -187,6 +217,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,15 +292,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>828040</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>2123440</xdr:rowOff>
+      <xdr:colOff>777240</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3952240</xdr:colOff>
+      <xdr:colOff>3901440</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>2085340</xdr:rowOff>
+      <xdr:rowOff>2212340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -290,8 +323,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7655560" y="9408160"/>
-          <a:ext cx="3124200" cy="2087880"/>
+          <a:off x="7597140" y="9133840"/>
+          <a:ext cx="3124200" cy="2082800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -347,15 +380,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
+      <xdr:colOff>152399</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
+      <xdr:rowOff>304799</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3035300</xdr:colOff>
+      <xdr:colOff>3177396</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1794498</xdr:rowOff>
+      <xdr:rowOff>1861068</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -378,8 +411,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2006600" y="5422900"/>
-          <a:ext cx="2895600" cy="1489698"/>
+          <a:off x="3586990" y="5416749"/>
+          <a:ext cx="3024997" cy="1556269"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -479,13 +512,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1003299</xdr:colOff>
+      <xdr:colOff>984343</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3962500</xdr:colOff>
+      <xdr:colOff>3943544</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>2159000</xdr:rowOff>
     </xdr:to>
@@ -510,7 +543,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7823199" y="3035300"/>
+          <a:off x="7808224" y="3027339"/>
           <a:ext cx="2959201" cy="1993900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -523,15 +556,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>927100</xdr:colOff>
+      <xdr:colOff>430143</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:rowOff>55770</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3797300</xdr:colOff>
+      <xdr:colOff>2334315</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>2065866</xdr:rowOff>
+      <xdr:rowOff>1325218</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -554,8 +587,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7747000" y="5270499"/>
-          <a:ext cx="2870200" cy="1913467"/>
+          <a:off x="7249491" y="5177183"/>
+          <a:ext cx="1904172" cy="1269448"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -567,15 +600,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>927100</xdr:colOff>
+      <xdr:colOff>317500</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>495300</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3956050</xdr:colOff>
+      <xdr:colOff>2489200</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2514600</xdr:rowOff>
+      <xdr:rowOff>1574800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -598,8 +631,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7747000" y="15100300"/>
-          <a:ext cx="3028950" cy="2019300"/>
+          <a:off x="7137400" y="14706600"/>
+          <a:ext cx="2171700" cy="1447800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -790,13 +823,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>204492</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>269068</xdr:rowOff>
+      <xdr:rowOff>288024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>3093997</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1765086</xdr:rowOff>
+      <xdr:rowOff>1784042</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -819,7 +852,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2066441" y="26519322"/>
+          <a:off x="3635388" y="28825114"/>
           <a:ext cx="2889505" cy="1496018"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1129,6 +1162,182 @@
         <a:xfrm>
           <a:off x="9385300" y="24701500"/>
           <a:ext cx="1828800" cy="1219200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2336800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1739900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4108450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2921000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD57FB02-25A8-674E-99D6-92E4D1D40F49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9156700" y="16319500"/>
+          <a:ext cx="1771650" cy="1181100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1090544</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>124239</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3615909</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1807816</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87CE5C26-73A8-9A4E-9DF3-DFAF144B1436}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7909892" y="7399130"/>
+          <a:ext cx="2525365" cy="1683577"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2595216</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>156452</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4431196</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1380438</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D126FC9-A9CD-8E42-98BF-B76790252016}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9414564" y="5277865"/>
+          <a:ext cx="1835980" cy="1223986"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>345109</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>538370</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3175000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1971995</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E7A075B-47BB-6441-B9EC-7D67B1F71997}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3768587" y="33737827"/>
+          <a:ext cx="2829891" cy="1433625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1437,11 +1646,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5A1329-3D34-824E-9BD6-BFD7C34C5F99}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="180" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="180" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1537,7 +1746,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3">
-        <v>184.8</v>
+        <v>189</v>
       </c>
       <c r="F4" s="3">
         <v>64000</v>
@@ -1546,27 +1755,29 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="154" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>210</v>
+      </c>
+      <c r="F5" s="3">
         <v>64000</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="166" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="188" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3" t="str">
-        <f>_xlfn.CONCAT(A6,".xslx")</f>
+        <f t="shared" ref="B6:B15" si="0">_xlfn.CONCAT(A6,".xslx")</f>
         <v>S01P5.xslx</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1588,7 +1799,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="str">
-        <f>_xlfn.CONCAT(A7,".xslx")</f>
+        <f t="shared" si="0"/>
         <v>S02P5.xslx</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1610,7 +1821,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="3" t="str">
-        <f>_xlfn.CONCAT(A8,".xslx")</f>
+        <f t="shared" si="0"/>
         <v>S03P5.xslx</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1632,7 +1843,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="str">
-        <f>_xlfn.CONCAT(A9,".xslx")</f>
+        <f t="shared" si="0"/>
         <v>C01P5.xslx</v>
       </c>
       <c r="C9" s="3"/>
@@ -1652,7 +1863,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="3" t="str">
-        <f>_xlfn.CONCAT(A10,".xslx")</f>
+        <f t="shared" si="0"/>
         <v>C02P5.xslx</v>
       </c>
       <c r="C10" s="3"/>
@@ -1668,7 +1879,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="3" t="str">
-        <f>_xlfn.CONCAT(A11,".xslx")</f>
+        <f t="shared" si="0"/>
         <v>S04P5.xslx</v>
       </c>
       <c r="C11" s="3"/>
@@ -1688,7 +1899,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="3" t="str">
-        <f>_xlfn.CONCAT(A12,".xslx")</f>
+        <f t="shared" si="0"/>
         <v>S05P2.xslx</v>
       </c>
       <c r="C12" s="3"/>
@@ -1708,7 +1919,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="3" t="str">
-        <f>_xlfn.CONCAT(A13,".xslx")</f>
+        <f t="shared" si="0"/>
         <v>S05P5.xslx</v>
       </c>
       <c r="C13" s="3"/>
@@ -1728,7 +1939,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="3" t="str">
-        <f>_xlfn.CONCAT(A14,".xslx")</f>
+        <f t="shared" si="0"/>
         <v>S05P10.xslx</v>
       </c>
       <c r="C14" s="3"/>
@@ -1742,6 +1953,15 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" ht="202" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>C03P5.xslx</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1751,15 +1971,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC721700-1AB0-104E-99BB-9F6A073030E6}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F21"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
         <v>9.5</v>
       </c>
@@ -1779,7 +1999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>9.5</v>
       </c>
@@ -1799,7 +2019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>9.5</v>
       </c>
@@ -1819,7 +2039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="23" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>8.5</v>
       </c>
@@ -1838,8 +2058,11 @@
       <c r="F4" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>8.5</v>
       </c>
@@ -1859,7 +2082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>7</v>
       </c>
@@ -1879,7 +2102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>7</v>
       </c>
@@ -1899,7 +2122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1919,7 +2142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -1939,7 +2162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -1959,7 +2182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>7</v>
       </c>
@@ -1979,7 +2202,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>7</v>
       </c>
@@ -1999,7 +2222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>7</v>
       </c>
@@ -2019,7 +2242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>7</v>
       </c>
@@ -2039,7 +2262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>7</v>
       </c>
@@ -2157,6 +2380,406 @@
       </c>
       <c r="F21" s="2">
         <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>0.39549600000000001</v>
+      </c>
+      <c r="C23">
+        <v>0.42494300000000002</v>
+      </c>
+      <c r="D23">
+        <v>0.85486300000000004</v>
+      </c>
+      <c r="E23">
+        <v>0.84495100000000001</v>
+      </c>
+      <c r="F23">
+        <v>0.52230500000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>0.320303</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0.38325399999999998</v>
+      </c>
+      <c r="E24">
+        <v>0.454816</v>
+      </c>
+      <c r="F24">
+        <v>0.65900599999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>0.68913599999999997</v>
+      </c>
+      <c r="C25">
+        <v>0.2</v>
+      </c>
+      <c r="D25">
+        <v>0.68906999999999996</v>
+      </c>
+      <c r="E25">
+        <v>0.84710099999999999</v>
+      </c>
+      <c r="F25">
+        <v>0.85395799999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0.993618</v>
+      </c>
+      <c r="B26">
+        <v>0.73308799999999996</v>
+      </c>
+      <c r="C26">
+        <v>0.2</v>
+      </c>
+      <c r="D26">
+        <v>0.65995099999999995</v>
+      </c>
+      <c r="E26">
+        <v>0.67742000000000002</v>
+      </c>
+      <c r="F26">
+        <v>0.393654</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>0.2</v>
+      </c>
+      <c r="B27">
+        <v>0.68372900000000003</v>
+      </c>
+      <c r="C27">
+        <v>0.62140200000000001</v>
+      </c>
+      <c r="D27">
+        <v>0.57374099999999995</v>
+      </c>
+      <c r="E27">
+        <v>0.2</v>
+      </c>
+      <c r="F27">
+        <v>0.54872399999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>0.67457599999999995</v>
+      </c>
+      <c r="B28">
+        <v>0.498921</v>
+      </c>
+      <c r="C28">
+        <v>0.93843100000000002</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0.33976899999999999</v>
+      </c>
+      <c r="F28">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>0.55446499999999999</v>
+      </c>
+      <c r="B29">
+        <v>0.2</v>
+      </c>
+      <c r="C29">
+        <v>0.2</v>
+      </c>
+      <c r="D29">
+        <v>0.91328399999999998</v>
+      </c>
+      <c r="E29">
+        <v>0.48861900000000003</v>
+      </c>
+      <c r="F29">
+        <v>0.88124800000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>0.51197599999999999</v>
+      </c>
+      <c r="B30">
+        <v>0.30038799999999999</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0.56914900000000002</v>
+      </c>
+      <c r="E30">
+        <v>0.2</v>
+      </c>
+      <c r="F30">
+        <v>0.57289500000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>0.2</v>
+      </c>
+      <c r="B31">
+        <v>0.65658399999999995</v>
+      </c>
+      <c r="C31">
+        <v>0.63422000000000001</v>
+      </c>
+      <c r="D31">
+        <v>0.67624899999999999</v>
+      </c>
+      <c r="E31">
+        <v>0.61883999999999995</v>
+      </c>
+      <c r="F31">
+        <v>0.632691</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>0.71615899999999999</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0.76386100000000001</v>
+      </c>
+      <c r="D32">
+        <v>0.35337200000000002</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0.60018899999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>3</v>
+      </c>
+      <c r="B34" s="2">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2">
+        <v>3</v>
+      </c>
+      <c r="F34" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>3</v>
+      </c>
+      <c r="B35" s="2">
+        <v>7</v>
+      </c>
+      <c r="C35" s="2">
+        <v>7</v>
+      </c>
+      <c r="D35" s="2">
+        <v>7</v>
+      </c>
+      <c r="E35" s="2">
+        <v>7</v>
+      </c>
+      <c r="F35" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>3</v>
+      </c>
+      <c r="B36" s="7">
+        <v>10</v>
+      </c>
+      <c r="C36" s="7">
+        <v>10</v>
+      </c>
+      <c r="D36" s="7">
+        <v>10</v>
+      </c>
+      <c r="E36" s="7">
+        <v>10</v>
+      </c>
+      <c r="F36" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>3</v>
+      </c>
+      <c r="B37" s="7">
+        <v>10</v>
+      </c>
+      <c r="C37" s="7">
+        <v>10</v>
+      </c>
+      <c r="D37" s="7">
+        <v>10</v>
+      </c>
+      <c r="E37" s="7">
+        <v>10</v>
+      </c>
+      <c r="F37" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>3</v>
+      </c>
+      <c r="B38" s="7">
+        <v>10</v>
+      </c>
+      <c r="C38" s="7">
+        <v>10</v>
+      </c>
+      <c r="D38" s="7">
+        <v>10</v>
+      </c>
+      <c r="E38" s="7">
+        <v>10</v>
+      </c>
+      <c r="F38" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>3</v>
+      </c>
+      <c r="B39" s="7">
+        <v>10</v>
+      </c>
+      <c r="C39" s="7">
+        <v>10</v>
+      </c>
+      <c r="D39" s="7">
+        <v>10</v>
+      </c>
+      <c r="E39" s="7">
+        <v>10</v>
+      </c>
+      <c r="F39" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>3</v>
+      </c>
+      <c r="B40" s="7">
+        <v>10</v>
+      </c>
+      <c r="C40" s="7">
+        <v>10</v>
+      </c>
+      <c r="D40" s="7">
+        <v>10</v>
+      </c>
+      <c r="E40" s="7">
+        <v>10</v>
+      </c>
+      <c r="F40" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>3</v>
+      </c>
+      <c r="B41" s="7">
+        <v>10</v>
+      </c>
+      <c r="C41" s="7">
+        <v>10</v>
+      </c>
+      <c r="D41" s="7">
+        <v>10</v>
+      </c>
+      <c r="E41" s="7">
+        <v>10</v>
+      </c>
+      <c r="F41" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>3</v>
+      </c>
+      <c r="B42" s="2">
+        <v>7</v>
+      </c>
+      <c r="C42" s="2">
+        <v>7</v>
+      </c>
+      <c r="D42" s="2">
+        <v>7</v>
+      </c>
+      <c r="E42" s="2">
+        <v>7</v>
+      </c>
+      <c r="F42" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>3</v>
+      </c>
+      <c r="B43" s="2">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2">
+        <v>3</v>
+      </c>
+      <c r="D43" s="2">
+        <v>3</v>
+      </c>
+      <c r="E43" s="2">
+        <v>3</v>
+      </c>
+      <c r="F43" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compared datasets against Series, TCT & SP.
Fixed Bypass Series connection as well. Some  brute force datasets perform better than TCT and SP, which is promising.
</commit_message>
<xml_diff>
--- a/Dataset Key.xlsx
+++ b/Dataset Key.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlima/Documents/GitHub/reconfigurable-solar-cells/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E711618F-B3BF-9E4E-A9CD-95A702DEEC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEE66D2-87CE-2344-92CE-524A0CD75CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{D03FEAF9-A323-DD42-AAE4-45997B47A029}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Shading Map Code</t>
   </si>
@@ -121,6 +121,9 @@
   <si>
     <t>C03P5</t>
   </si>
+  <si>
+    <t>Bypass</t>
+  </si>
 </sst>
 </file>
 
@@ -170,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -193,22 +196,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -219,7 +211,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,13 +635,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
+      <xdr:colOff>574676</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4191000</xdr:colOff>
+      <xdr:colOff>4206876</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>2599267</xdr:rowOff>
     </xdr:to>
@@ -675,7 +666,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7378700" y="17843500"/>
+          <a:off x="7392989" y="17830800"/>
           <a:ext cx="3632200" cy="2421467"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -823,13 +814,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>204492</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>288024</xdr:rowOff>
+      <xdr:rowOff>298607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>3093997</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1784042</xdr:rowOff>
+      <xdr:rowOff>1794625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -852,7 +843,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3635388" y="28825114"/>
+          <a:off x="3633492" y="29021774"/>
           <a:ext cx="2889505" cy="1496018"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -909,13 +900,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>781538</xdr:colOff>
+      <xdr:colOff>790005</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>93039</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4244313</xdr:colOff>
+      <xdr:colOff>4252780</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>2401556</xdr:rowOff>
     </xdr:to>
@@ -940,7 +931,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7606043" y="28340072"/>
+          <a:off x="7622605" y="30843972"/>
           <a:ext cx="3462775" cy="2308517"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1261,15 +1252,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2595216</xdr:colOff>
+      <xdr:colOff>2586046</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>156452</xdr:rowOff>
+      <xdr:rowOff>92265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4431196</xdr:colOff>
+      <xdr:colOff>4422026</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1380438</xdr:rowOff>
+      <xdr:rowOff>1316251</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1292,7 +1283,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9414564" y="5277865"/>
+          <a:off x="9408284" y="5208944"/>
           <a:ext cx="1835980" cy="1223986"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1338,6 +1329,50 @@
         <a:xfrm>
           <a:off x="3768587" y="33737827"/>
           <a:ext cx="2829891" cy="1433625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>759239</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>151848</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4099891</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2378949</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C46CBAC7-2B51-064C-B66A-322DD02062E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7578587" y="33351305"/>
+          <a:ext cx="3340652" cy="2227101"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1646,11 +1681,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5A1329-3D34-824E-9BD6-BFD7C34C5F99}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="180" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1662,7 +1697,7 @@
     <col min="5" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1685,13 +1720,16 @@
         <v>19</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1709,11 +1747,20 @@
       <c r="F2" s="3">
         <v>64000</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G2" s="3">
+        <v>127.38</v>
+      </c>
+      <c r="H2" s="3">
+        <v>127.38</v>
+      </c>
+      <c r="I2" s="3">
+        <v>222.48</v>
+      </c>
+      <c r="J2" s="3">
+        <v>200.59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1731,11 +1778,20 @@
       <c r="F3" s="3">
         <v>125000</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="3">
+        <v>127.38</v>
+      </c>
+      <c r="H3" s="3">
+        <v>127.38</v>
+      </c>
+      <c r="I3" s="3">
+        <v>222.48</v>
+      </c>
+      <c r="J3" s="3">
+        <v>200.59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1751,11 +1807,20 @@
       <c r="F4" s="3">
         <v>64000</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G4" s="3">
+        <v>86.13</v>
+      </c>
+      <c r="H4" s="3">
+        <v>86.13</v>
+      </c>
+      <c r="I4" s="3">
+        <v>227.83</v>
+      </c>
+      <c r="J4" s="3">
+        <v>104.28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1768,11 +1833,20 @@
       <c r="F5" s="3">
         <v>64000</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="188" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="3">
+        <v>86.13</v>
+      </c>
+      <c r="H5" s="3">
+        <v>86.13</v>
+      </c>
+      <c r="I5" s="3">
+        <v>227.83</v>
+      </c>
+      <c r="J5" s="3">
+        <v>104.28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="188" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1790,11 +1864,20 @@
       <c r="F6" s="3">
         <v>64000</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G6" s="3">
+        <v>128.66</v>
+      </c>
+      <c r="H6" s="3">
+        <v>128.66</v>
+      </c>
+      <c r="I6" s="3">
+        <v>128.65</v>
+      </c>
+      <c r="J6" s="3">
+        <v>128.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1812,11 +1895,20 @@
       <c r="F7" s="3">
         <v>64000</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G7" s="3">
+        <v>130.38999999999999</v>
+      </c>
+      <c r="H7" s="3">
+        <v>216.72</v>
+      </c>
+      <c r="I7" s="3">
+        <v>254.27</v>
+      </c>
+      <c r="J7" s="3">
+        <v>254.27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1834,11 +1926,20 @@
       <c r="F8" s="3">
         <v>64000</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="224" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G8" s="3">
+        <v>128.66</v>
+      </c>
+      <c r="H8" s="3">
+        <v>128.66</v>
+      </c>
+      <c r="I8" s="3">
+        <v>128.65</v>
+      </c>
+      <c r="J8" s="3">
+        <v>128.65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="224" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -1854,11 +1955,20 @@
       <c r="F9" s="3">
         <v>64000</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="223" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G9" s="3">
+        <v>103.73</v>
+      </c>
+      <c r="H9" s="3">
+        <v>103.73</v>
+      </c>
+      <c r="I9" s="3">
+        <v>181.75</v>
+      </c>
+      <c r="J9" s="3">
+        <v>159.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="223" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1868,13 +1978,26 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="229" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="3">
+        <v>169</v>
+      </c>
+      <c r="F10" s="3">
+        <v>64000</v>
+      </c>
+      <c r="G10" s="3">
+        <v>81.209999999999994</v>
+      </c>
+      <c r="H10" s="3">
+        <v>81.209999999999994</v>
+      </c>
+      <c r="I10" s="3">
+        <v>204.76</v>
+      </c>
+      <c r="J10" s="3">
+        <v>81.209999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="229" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1890,11 +2013,20 @@
       <c r="F11" s="3">
         <v>64000</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G11" s="3">
+        <v>121.41</v>
+      </c>
+      <c r="H11" s="3">
+        <v>121.41</v>
+      </c>
+      <c r="I11" s="3">
+        <v>190.98</v>
+      </c>
+      <c r="J11" s="3">
+        <v>119.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1910,11 +2042,20 @@
       <c r="F12" s="3">
         <v>64000</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="157" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G12" s="3">
+        <v>87.9</v>
+      </c>
+      <c r="H12" s="3">
+        <v>87.91</v>
+      </c>
+      <c r="I12" s="3">
+        <v>192.71</v>
+      </c>
+      <c r="J12" s="3">
+        <v>190.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="157" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1930,11 +2071,20 @@
       <c r="F13" s="3">
         <v>64000</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="196" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G13" s="3">
+        <v>87.9</v>
+      </c>
+      <c r="H13" s="3">
+        <v>27.04</v>
+      </c>
+      <c r="I13" s="3">
+        <v>192.71</v>
+      </c>
+      <c r="J13" s="3">
+        <v>190.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="196" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1950,17 +2100,46 @@
       <c r="F14" s="3">
         <v>64000</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="202" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="G14" s="3">
+        <v>87.9</v>
+      </c>
+      <c r="H14" s="3">
+        <v>27.04</v>
+      </c>
+      <c r="I14" s="3">
+        <v>192.71</v>
+      </c>
+      <c r="J14" s="3">
+        <v>190.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="202" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="8" t="str">
+      <c r="B15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>C03P5.xslx</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3">
+        <v>215</v>
+      </c>
+      <c r="F15" s="3">
+        <v>64000</v>
+      </c>
+      <c r="G15" s="3">
+        <v>123.07</v>
+      </c>
+      <c r="H15" s="3">
+        <v>123.07</v>
+      </c>
+      <c r="I15" s="3">
+        <v>125.47</v>
+      </c>
+      <c r="J15" s="3">
+        <v>119.77</v>
       </c>
     </row>
   </sheetData>
@@ -1971,37 +2150,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC721700-1AB0-104E-99BB-9F6A073030E6}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:F43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2">
         <v>9.5</v>
       </c>
       <c r="D1" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="E1" s="2">
         <v>8.5</v>
       </c>
-      <c r="E1" s="2">
-        <v>7</v>
-      </c>
       <c r="F1" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>9.5</v>
@@ -2013,10 +2192,10 @@
         <v>8.5</v>
       </c>
       <c r="E2" s="2">
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="F2" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2027,21 +2206,21 @@
         <v>9.5</v>
       </c>
       <c r="C3" s="2">
-        <v>9.5</v>
+        <v>8.5</v>
       </c>
       <c r="D3" s="2">
         <v>8.5</v>
       </c>
       <c r="E3" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="23" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="B4" s="2">
         <v>8.5</v>
@@ -2053,7 +2232,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2">
         <v>5</v>
@@ -2073,7 +2252,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="2">
         <v>5</v>
@@ -2084,13 +2263,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>7</v>
       </c>
       <c r="C6" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2">
         <v>5</v>
@@ -2099,7 +2278,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2107,7 +2286,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
         <v>5</v>
@@ -2116,21 +2295,21 @@
         <v>5</v>
       </c>
       <c r="E7" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2">
         <v>4</v>
@@ -2139,41 +2318,41 @@
         <v>4</v>
       </c>
       <c r="F8" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
-        <v>3</v>
-      </c>
       <c r="D9" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="2">
         <v>3</v>
       </c>
       <c r="F9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
@@ -2780,6 +2959,206 @@
       </c>
       <c r="F43" s="2">
         <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D45" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E45" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F45" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>5</v>
+      </c>
+      <c r="B46" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D46" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E46" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F46" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>5</v>
+      </c>
+      <c r="B47" s="7">
+        <v>7</v>
+      </c>
+      <c r="C47" s="7">
+        <v>7</v>
+      </c>
+      <c r="D47" s="7">
+        <v>7</v>
+      </c>
+      <c r="E47" s="7">
+        <v>7</v>
+      </c>
+      <c r="F47" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>5</v>
+      </c>
+      <c r="B48" s="7">
+        <v>7</v>
+      </c>
+      <c r="C48" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="D48" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="E48" s="7">
+        <v>7</v>
+      </c>
+      <c r="F48" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>5</v>
+      </c>
+      <c r="B49" s="7">
+        <v>7</v>
+      </c>
+      <c r="C49" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="D49" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="E49" s="7">
+        <v>7</v>
+      </c>
+      <c r="F49" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>5</v>
+      </c>
+      <c r="B50" s="7">
+        <v>7</v>
+      </c>
+      <c r="C50" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="D50" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="E50" s="7">
+        <v>7</v>
+      </c>
+      <c r="F50" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>5</v>
+      </c>
+      <c r="B51" s="7">
+        <v>7</v>
+      </c>
+      <c r="C51" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="D51" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="E51" s="7">
+        <v>7</v>
+      </c>
+      <c r="F51" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>5</v>
+      </c>
+      <c r="B52" s="7">
+        <v>7</v>
+      </c>
+      <c r="C52" s="7">
+        <v>7</v>
+      </c>
+      <c r="D52" s="7">
+        <v>7</v>
+      </c>
+      <c r="E52" s="7">
+        <v>7</v>
+      </c>
+      <c r="F52" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>5</v>
+      </c>
+      <c r="B53" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C53" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D53" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E53" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F53" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="B54" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C54" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D54" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E54" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F54" s="2">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added triangular shading maps
Errors occurred when no current was generated. Added an if statement to continue loop in this event rather than throw an error.
</commit_message>
<xml_diff>
--- a/Dataset Key.xlsx
+++ b/Dataset Key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlima/Documents/GitHub/reconfigurable-solar-cells/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEE66D2-87CE-2344-92CE-524A0CD75CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56617E91-D929-934F-9DB5-143C6B3F9805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{D03FEAF9-A323-DD42-AAE4-45997B47A029}"/>
+    <workbookView xWindow="30240" yWindow="-10060" windowWidth="38400" windowHeight="21100" xr2:uid="{D03FEAF9-A323-DD42-AAE4-45997B47A029}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Shading Map Code</t>
   </si>
@@ -124,12 +124,30 @@
   <si>
     <t>Bypass</t>
   </si>
+  <si>
+    <t>M01P5</t>
+  </si>
+  <si>
+    <t>Upper Triangular</t>
+  </si>
+  <si>
+    <t>Lower Triangular</t>
+  </si>
+  <si>
+    <t>T01P5</t>
+  </si>
+  <si>
+    <t>T02P5</t>
+  </si>
+  <si>
+    <t>Improvement</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +176,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -168,7 +193,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -197,25 +222,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -622,7 +661,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7137400" y="14706600"/>
+          <a:off x="7136423" y="14702692"/>
           <a:ext cx="2171700" cy="1447800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1195,7 +1234,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9156700" y="16319500"/>
+          <a:off x="9155723" y="16315592"/>
           <a:ext cx="1771650" cy="1181100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1283,7 +1322,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9408284" y="5208944"/>
+          <a:off x="9404969" y="5211342"/>
           <a:ext cx="1835980" cy="1223986"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1373,6 +1412,181 @@
         <a:xfrm>
           <a:off x="7578587" y="33351305"/>
           <a:ext cx="3340652" cy="2227101"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>924560</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>358986</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3891280</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>2336799</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94F84912-651C-9C91-AC86-036064593452}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7752080" y="36142506"/>
+          <a:ext cx="2966720" cy="1977813"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>81280</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>538480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3271520</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>2153920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF4FC760-E9E4-7DEC-3114-B0954D661C9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:srcRect l="-1" r="1582"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3515360" y="36322000"/>
+          <a:ext cx="3190240" cy="1615440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>67732</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4074160</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2438399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73720753-0D62-AD52-0F15-E4CFAD084B76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7345680" y="38899252"/>
+          <a:ext cx="3556000" cy="2370667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>721360</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>64346</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3749040</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2082799</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD3D47CC-01C4-9C1B-DF0F-5040D50668C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7548880" y="38692666"/>
+          <a:ext cx="3027680" cy="2018453"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1681,468 +1895,639 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5A1329-3D34-824E-9BD6-BFD7C34C5F99}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="44.5" customWidth="1"/>
-    <col min="4" max="4" width="60.33203125" customWidth="1"/>
-    <col min="5" max="6" width="21" customWidth="1"/>
+    <col min="1" max="1" width="24.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="44.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="60.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="5" customWidth="1"/>
+    <col min="6" max="9" width="10.83203125" style="5"/>
+    <col min="10" max="10" width="15.83203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="21" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="210" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="str">
+      <c r="B2" s="6" t="str">
         <f>_xlfn.CONCAT(A2,".xslx")</f>
         <v>B9378P5.xslx</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6">
         <v>202.3</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="6">
+        <v>127.38</v>
+      </c>
+      <c r="G2" s="6">
+        <v>127.38</v>
+      </c>
+      <c r="H2" s="6">
+        <v>222.48</v>
+      </c>
+      <c r="I2" s="6">
+        <v>200.59</v>
+      </c>
+      <c r="J2" s="7">
+        <f>E2/MAX(F2:I2)</f>
+        <v>0.90929521754764486</v>
+      </c>
+      <c r="K2" s="6">
         <v>64000</v>
       </c>
-      <c r="G2" s="3">
-        <v>127.38</v>
-      </c>
-      <c r="H2" s="3">
-        <v>127.38</v>
-      </c>
-      <c r="I2" s="3">
-        <v>222.48</v>
-      </c>
-      <c r="J2" s="3">
-        <v>200.59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="3" spans="1:11" ht="177" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="str">
+      <c r="B3" s="6" t="str">
         <f>_xlfn.CONCAT(A3,".xslx")</f>
         <v>B9378P10.xslx</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6">
         <v>229.7</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="6">
+        <v>127.38</v>
+      </c>
+      <c r="G3" s="6">
+        <v>127.38</v>
+      </c>
+      <c r="H3" s="6">
+        <v>222.48</v>
+      </c>
+      <c r="I3" s="6">
+        <v>200.59</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" ref="J3:J18" si="0">E3/MAX(F3:I3)</f>
+        <v>1.0324523552678893</v>
+      </c>
+      <c r="K3" s="6">
         <v>125000</v>
       </c>
-      <c r="G3" s="3">
-        <v>127.38</v>
-      </c>
-      <c r="H3" s="3">
-        <v>127.38</v>
-      </c>
-      <c r="I3" s="3">
-        <v>222.48</v>
-      </c>
-      <c r="J3" s="3">
-        <v>200.59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="str">
+    </row>
+    <row r="4" spans="1:11" ht="170" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6" t="str">
         <f>_xlfn.CONCAT(A4,".xslx")</f>
         <v>﻿R01P5.xslx</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6">
         <v>189</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
+        <v>86.13</v>
+      </c>
+      <c r="G4" s="6">
+        <v>86.13</v>
+      </c>
+      <c r="H4" s="6">
+        <v>227.83</v>
+      </c>
+      <c r="I4" s="6">
+        <v>104.28</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.8295659044024053</v>
+      </c>
+      <c r="K4" s="6">
         <v>64000</v>
       </c>
-      <c r="G4" s="3">
+    </row>
+    <row r="5" spans="1:11" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6">
+        <v>210</v>
+      </c>
+      <c r="F5" s="6">
         <v>86.13</v>
       </c>
-      <c r="H4" s="3">
+      <c r="G5" s="6">
         <v>86.13</v>
       </c>
-      <c r="I4" s="3">
+      <c r="H5" s="6">
         <v>227.83</v>
       </c>
-      <c r="J4" s="3">
+      <c r="I5" s="6">
         <v>104.28</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="146" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3">
-        <v>210</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="J5" s="7">
+        <f t="shared" si="0"/>
+        <v>0.92173989378045029</v>
+      </c>
+      <c r="K5" s="6">
         <v>64000</v>
       </c>
-      <c r="G5" s="3">
-        <v>86.13</v>
-      </c>
-      <c r="H5" s="3">
-        <v>86.13</v>
-      </c>
-      <c r="I5" s="3">
-        <v>227.83</v>
-      </c>
-      <c r="J5" s="3">
-        <v>104.28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="188" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    </row>
+    <row r="6" spans="1:11" ht="188" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="str">
-        <f t="shared" ref="B6:B15" si="0">_xlfn.CONCAT(A6,".xslx")</f>
+      <c r="B6" s="6" t="str">
+        <f t="shared" ref="B6:B18" si="1">_xlfn.CONCAT(A6,".xslx")</f>
         <v>S01P5.xslx</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6">
         <v>230</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
+        <v>128.66</v>
+      </c>
+      <c r="G6" s="6">
+        <v>128.66</v>
+      </c>
+      <c r="H6" s="6">
+        <v>128.65</v>
+      </c>
+      <c r="I6" s="6">
+        <v>128.65</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="0"/>
+        <v>1.7876573915746929</v>
+      </c>
+      <c r="K6" s="6">
         <v>64000</v>
       </c>
-      <c r="G6" s="3">
+    </row>
+    <row r="7" spans="1:11" ht="241" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>S02P5.xslx</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6">
+        <v>202</v>
+      </c>
+      <c r="F7" s="6">
+        <v>130.38999999999999</v>
+      </c>
+      <c r="G7" s="6">
+        <v>216.72</v>
+      </c>
+      <c r="H7" s="6">
+        <v>254.27</v>
+      </c>
+      <c r="I7" s="6">
+        <v>254.27</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="0"/>
+        <v>0.79443111652967313</v>
+      </c>
+      <c r="K7" s="6">
+        <v>64000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="241" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>S03P5.xslx</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6">
+        <v>219</v>
+      </c>
+      <c r="F8" s="6">
         <v>128.66</v>
       </c>
-      <c r="H6" s="3">
+      <c r="G8" s="6">
         <v>128.66</v>
       </c>
-      <c r="I6" s="3">
+      <c r="H8" s="6">
         <v>128.65</v>
       </c>
-      <c r="J6" s="3">
+      <c r="I8" s="6">
         <v>128.65</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="str">
+      <c r="J8" s="7">
         <f t="shared" si="0"/>
-        <v>S02P5.xslx</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3">
-        <v>202</v>
-      </c>
-      <c r="F7" s="3">
+        <v>1.702160733716773</v>
+      </c>
+      <c r="K8" s="6">
         <v>64000</v>
       </c>
-      <c r="G7" s="3">
-        <v>130.38999999999999</v>
-      </c>
-      <c r="H7" s="3">
-        <v>216.72</v>
-      </c>
-      <c r="I7" s="3">
-        <v>254.27</v>
-      </c>
-      <c r="J7" s="3">
-        <v>254.27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="241" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="3" t="str">
+    </row>
+    <row r="9" spans="1:11" ht="224" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>C01P5.xslx</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6">
+        <v>146</v>
+      </c>
+      <c r="F9" s="6">
+        <v>103.73</v>
+      </c>
+      <c r="G9" s="6">
+        <v>103.73</v>
+      </c>
+      <c r="H9" s="6">
+        <v>181.75</v>
+      </c>
+      <c r="I9" s="6">
+        <v>159.16</v>
+      </c>
+      <c r="J9" s="7">
         <f t="shared" si="0"/>
-        <v>S03P5.xslx</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3">
-        <v>219</v>
-      </c>
-      <c r="F8" s="3">
+        <v>0.80330123796423658</v>
+      </c>
+      <c r="K9" s="6">
         <v>64000</v>
       </c>
-      <c r="G8" s="3">
-        <v>128.66</v>
-      </c>
-      <c r="H8" s="3">
-        <v>128.66</v>
-      </c>
-      <c r="I8" s="3">
-        <v>128.65</v>
-      </c>
-      <c r="J8" s="3">
-        <v>128.65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="224" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="str">
+    </row>
+    <row r="10" spans="1:11" ht="223" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>C02P5.xslx</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6">
+        <v>169</v>
+      </c>
+      <c r="F10" s="6">
+        <v>81.209999999999994</v>
+      </c>
+      <c r="G10" s="6">
+        <v>81.209999999999994</v>
+      </c>
+      <c r="H10" s="6">
+        <v>204.76</v>
+      </c>
+      <c r="I10" s="6">
+        <v>81.209999999999994</v>
+      </c>
+      <c r="J10" s="7">
         <f t="shared" si="0"/>
-        <v>C01P5.xslx</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3">
-        <v>146</v>
-      </c>
-      <c r="F9" s="3">
+        <v>0.82535651494432505</v>
+      </c>
+      <c r="K10" s="6">
         <v>64000</v>
       </c>
-      <c r="G9" s="3">
-        <v>103.73</v>
-      </c>
-      <c r="H9" s="3">
-        <v>103.73</v>
-      </c>
-      <c r="I9" s="3">
-        <v>181.75</v>
-      </c>
-      <c r="J9" s="3">
-        <v>159.16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="223" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="3" t="str">
+    </row>
+    <row r="11" spans="1:11" ht="229" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>S04P5.xslx</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6">
+        <v>170</v>
+      </c>
+      <c r="F11" s="6">
+        <v>121.41</v>
+      </c>
+      <c r="G11" s="6">
+        <v>121.41</v>
+      </c>
+      <c r="H11" s="6">
+        <v>190.98</v>
+      </c>
+      <c r="I11" s="6">
+        <v>119.52</v>
+      </c>
+      <c r="J11" s="7">
         <f t="shared" si="0"/>
-        <v>C02P5.xslx</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3">
-        <v>169</v>
-      </c>
-      <c r="F10" s="3">
+        <v>0.89014556498062625</v>
+      </c>
+      <c r="K11" s="6">
         <v>64000</v>
       </c>
-      <c r="G10" s="3">
-        <v>81.209999999999994</v>
-      </c>
-      <c r="H10" s="3">
-        <v>81.209999999999994</v>
-      </c>
-      <c r="I10" s="3">
-        <v>204.76</v>
-      </c>
-      <c r="J10" s="3">
-        <v>81.209999999999994</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="229" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3" t="str">
+    </row>
+    <row r="12" spans="1:11" ht="197" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>S05P2.xslx</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6">
+        <v>225</v>
+      </c>
+      <c r="F12" s="6">
+        <v>87.9</v>
+      </c>
+      <c r="G12" s="6">
+        <v>87.91</v>
+      </c>
+      <c r="H12" s="6">
+        <v>192.71</v>
+      </c>
+      <c r="I12" s="6">
+        <v>190.95</v>
+      </c>
+      <c r="J12" s="7">
         <f t="shared" si="0"/>
-        <v>S04P5.xslx</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3">
-        <v>170</v>
-      </c>
-      <c r="F11" s="3">
+        <v>1.1675574697732343</v>
+      </c>
+      <c r="K12" s="6">
         <v>64000</v>
       </c>
-      <c r="G11" s="3">
-        <v>121.41</v>
-      </c>
-      <c r="H11" s="3">
-        <v>121.41</v>
-      </c>
-      <c r="I11" s="3">
-        <v>190.98</v>
-      </c>
-      <c r="J11" s="3">
-        <v>119.52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="3" t="str">
+    </row>
+    <row r="13" spans="1:11" ht="157" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>S05P5.xslx</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6">
+        <v>209</v>
+      </c>
+      <c r="F13" s="6">
+        <v>87.9</v>
+      </c>
+      <c r="G13" s="6">
+        <v>27.04</v>
+      </c>
+      <c r="H13" s="6">
+        <v>192.71</v>
+      </c>
+      <c r="I13" s="6">
+        <v>190.95</v>
+      </c>
+      <c r="J13" s="7">
         <f t="shared" si="0"/>
-        <v>S05P2.xslx</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3">
-        <v>225</v>
-      </c>
-      <c r="F12" s="3">
+        <v>1.0845311608115822</v>
+      </c>
+      <c r="K13" s="6">
         <v>64000</v>
       </c>
-      <c r="G12" s="3">
+    </row>
+    <row r="14" spans="1:11" ht="196" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>S05P10.xslx</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6">
+        <v>192</v>
+      </c>
+      <c r="F14" s="6">
         <v>87.9</v>
       </c>
-      <c r="H12" s="3">
-        <v>87.91</v>
-      </c>
-      <c r="I12" s="3">
+      <c r="G14" s="6">
+        <v>27.04</v>
+      </c>
+      <c r="H14" s="6">
         <v>192.71</v>
       </c>
-      <c r="J12" s="3">
+      <c r="I14" s="6">
         <v>190.95</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="157" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="3" t="str">
+      <c r="J14" s="7">
         <f t="shared" si="0"/>
-        <v>S05P5.xslx</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3">
-        <v>209</v>
-      </c>
-      <c r="F13" s="3">
+        <v>0.99631570753982668</v>
+      </c>
+      <c r="K14" s="6">
         <v>64000</v>
       </c>
-      <c r="G13" s="3">
-        <v>87.9</v>
-      </c>
-      <c r="H13" s="3">
-        <v>27.04</v>
-      </c>
-      <c r="I13" s="3">
-        <v>192.71</v>
-      </c>
-      <c r="J13" s="3">
-        <v>190.95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="196" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="3" t="str">
+    </row>
+    <row r="15" spans="1:11" ht="202" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>C03P5.xslx</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6">
+        <v>215</v>
+      </c>
+      <c r="F15" s="6">
+        <v>123.07</v>
+      </c>
+      <c r="G15" s="6">
+        <v>123.07</v>
+      </c>
+      <c r="H15" s="6">
+        <v>125.47</v>
+      </c>
+      <c r="I15" s="6">
+        <v>119.77</v>
+      </c>
+      <c r="J15" s="7">
         <f t="shared" si="0"/>
-        <v>S05P10.xslx</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3">
-        <v>192</v>
-      </c>
-      <c r="F14" s="3">
+        <v>1.7135570255838048</v>
+      </c>
+      <c r="K15" s="6">
         <v>64000</v>
       </c>
-      <c r="G14" s="3">
-        <v>87.9</v>
-      </c>
-      <c r="H14" s="3">
-        <v>27.04</v>
-      </c>
-      <c r="I14" s="3">
-        <v>192.71</v>
-      </c>
-      <c r="J14" s="3">
-        <v>190.95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="202" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="3" t="str">
+    </row>
+    <row r="16" spans="1:11" ht="224" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>M01P5.xslx</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6">
+        <v>370</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <v>234.99</v>
+      </c>
+      <c r="H16" s="6">
+        <v>364.68</v>
+      </c>
+      <c r="I16" s="6">
+        <v>311.69</v>
+      </c>
+      <c r="J16" s="7">
         <f t="shared" si="0"/>
-        <v>C03P5.xslx</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3">
-        <v>215</v>
-      </c>
-      <c r="F15" s="3">
+        <v>1.0145881320609849</v>
+      </c>
+      <c r="K16" s="6">
         <v>64000</v>
       </c>
-      <c r="G15" s="3">
-        <v>123.07</v>
-      </c>
-      <c r="H15" s="3">
-        <v>123.07</v>
-      </c>
-      <c r="I15" s="3">
-        <v>125.47</v>
-      </c>
-      <c r="J15" s="3">
-        <v>119.77</v>
+    </row>
+    <row r="17" spans="1:11" ht="169" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>T01P5.xslx</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6">
+        <v>119</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>42.14</v>
+      </c>
+      <c r="I17" s="6">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="0"/>
+        <v>2.823920265780731</v>
+      </c>
+      <c r="K17" s="6">
+        <v>64000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="198" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>T02P5.xslx</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6">
+        <v>233</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+      <c r="G18" s="6">
+        <v>157.69999999999999</v>
+      </c>
+      <c r="H18" s="6">
+        <v>211.74</v>
+      </c>
+      <c r="I18" s="6">
+        <v>194.15</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="0"/>
+        <v>1.100406158496269</v>
+      </c>
+      <c r="K18" s="6">
+        <v>64000</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2159,405 +2544,405 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2">
+      <c r="A1" s="1">
         <v>10</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>10</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="1">
         <v>9.5</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <v>9.5</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="1">
         <v>8.5</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>9.5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>9.5</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>8.5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>8.5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>9.5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>9.5</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>8.5</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>8.5</v>
       </c>
-      <c r="E3" s="2">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="1">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="23" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>9.5</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>8.5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>8.5</v>
       </c>
-      <c r="D4" s="2">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4" s="1">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
         <v>6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>5</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>8.5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>8.5</v>
       </c>
-      <c r="C5" s="2">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
         <v>6</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>5</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>8</v>
       </c>
-      <c r="B6" s="2">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>5</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>4</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>5</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>4</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>4</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>5</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>4</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>4</v>
       </c>
-      <c r="E9" s="2">
-        <v>3</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>5</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>4</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>4</v>
       </c>
-      <c r="D10" s="2">
-        <v>3</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2">
-        <v>7</v>
-      </c>
-      <c r="D12" s="2">
-        <v>7</v>
-      </c>
-      <c r="E12" s="2">
-        <v>7</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="A12" s="1">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2">
-        <v>3</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="A13" s="1">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>7</v>
-      </c>
-      <c r="B14" s="2">
-        <v>7</v>
-      </c>
-      <c r="C14" s="2">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2">
-        <v>3</v>
-      </c>
-      <c r="E14" s="2">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2">
-        <v>7</v>
-      </c>
-      <c r="C15" s="2">
-        <v>3</v>
-      </c>
-      <c r="D15" s="2">
-        <v>3</v>
-      </c>
-      <c r="E15" s="2">
-        <v>3</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="A15" s="1">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2">
-        <v>3</v>
-      </c>
-      <c r="D16" s="2">
-        <v>3</v>
-      </c>
-      <c r="E16" s="2">
-        <v>3</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="A16" s="1">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>3</v>
-      </c>
-      <c r="B17" s="2">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2">
-        <v>3</v>
-      </c>
-      <c r="D17" s="2">
-        <v>3</v>
-      </c>
-      <c r="E17" s="2">
-        <v>3</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>3</v>
-      </c>
-      <c r="B18" s="2">
-        <v>3</v>
-      </c>
-      <c r="C18" s="2">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2">
-        <v>3</v>
-      </c>
-      <c r="E18" s="2">
-        <v>7</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>3</v>
-      </c>
-      <c r="B19" s="2">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2">
-        <v>3</v>
-      </c>
-      <c r="D19" s="2">
-        <v>7</v>
-      </c>
-      <c r="E19" s="2">
-        <v>7</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="A19" s="1">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1">
+        <v>7</v>
+      </c>
+      <c r="F19" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2">
-        <v>3</v>
-      </c>
-      <c r="C20" s="2">
-        <v>7</v>
-      </c>
-      <c r="D20" s="2">
-        <v>7</v>
-      </c>
-      <c r="E20" s="2">
-        <v>7</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="A20" s="1">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>3</v>
-      </c>
-      <c r="B21" s="2">
-        <v>7</v>
-      </c>
-      <c r="C21" s="2">
-        <v>7</v>
-      </c>
-      <c r="D21" s="2">
-        <v>7</v>
-      </c>
-      <c r="E21" s="2">
-        <v>7</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1">
+        <v>7</v>
+      </c>
+      <c r="F21" s="1">
         <v>7</v>
       </c>
     </row>
@@ -2762,402 +3147,402 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
-        <v>3</v>
-      </c>
-      <c r="B34" s="2">
-        <v>3</v>
-      </c>
-      <c r="C34" s="2">
-        <v>3</v>
-      </c>
-      <c r="D34" s="2">
-        <v>3</v>
-      </c>
-      <c r="E34" s="2">
-        <v>3</v>
-      </c>
-      <c r="F34" s="2">
+      <c r="A34" s="1">
+        <v>3</v>
+      </c>
+      <c r="B34" s="1">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1">
+        <v>3</v>
+      </c>
+      <c r="F34" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
-        <v>3</v>
-      </c>
-      <c r="B35" s="2">
-        <v>7</v>
-      </c>
-      <c r="C35" s="2">
-        <v>7</v>
-      </c>
-      <c r="D35" s="2">
-        <v>7</v>
-      </c>
-      <c r="E35" s="2">
-        <v>7</v>
-      </c>
-      <c r="F35" s="2">
+      <c r="A35" s="1">
+        <v>3</v>
+      </c>
+      <c r="B35" s="1">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1">
+        <v>7</v>
+      </c>
+      <c r="D35" s="1">
+        <v>7</v>
+      </c>
+      <c r="E35" s="1">
+        <v>7</v>
+      </c>
+      <c r="F35" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
-        <v>3</v>
-      </c>
-      <c r="B36" s="7">
+      <c r="A36" s="1">
+        <v>3</v>
+      </c>
+      <c r="B36" s="3">
         <v>10</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="3">
         <v>10</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="3">
         <v>10</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="3">
         <v>10</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
-        <v>3</v>
-      </c>
-      <c r="B37" s="7">
+      <c r="A37" s="1">
+        <v>3</v>
+      </c>
+      <c r="B37" s="3">
         <v>10</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="3">
         <v>10</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="3">
         <v>10</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="3">
         <v>10</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>3</v>
-      </c>
-      <c r="B38" s="7">
+      <c r="A38" s="1">
+        <v>3</v>
+      </c>
+      <c r="B38" s="3">
         <v>10</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="3">
         <v>10</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="3">
         <v>10</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="3">
         <v>10</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
-        <v>3</v>
-      </c>
-      <c r="B39" s="7">
+      <c r="A39" s="1">
+        <v>3</v>
+      </c>
+      <c r="B39" s="3">
         <v>10</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="3">
         <v>10</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="3">
         <v>10</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="3">
         <v>10</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
-        <v>3</v>
-      </c>
-      <c r="B40" s="7">
+      <c r="A40" s="1">
+        <v>3</v>
+      </c>
+      <c r="B40" s="3">
         <v>10</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="3">
         <v>10</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="3">
         <v>10</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="3">
         <v>10</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
-        <v>3</v>
-      </c>
-      <c r="B41" s="7">
+      <c r="A41" s="1">
+        <v>3</v>
+      </c>
+      <c r="B41" s="3">
         <v>10</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="3">
         <v>10</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="3">
         <v>10</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="3">
         <v>10</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
-        <v>3</v>
-      </c>
-      <c r="B42" s="2">
-        <v>7</v>
-      </c>
-      <c r="C42" s="2">
-        <v>7</v>
-      </c>
-      <c r="D42" s="2">
-        <v>7</v>
-      </c>
-      <c r="E42" s="2">
-        <v>7</v>
-      </c>
-      <c r="F42" s="2">
+      <c r="A42" s="1">
+        <v>3</v>
+      </c>
+      <c r="B42" s="1">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1">
+        <v>7</v>
+      </c>
+      <c r="F42" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
-        <v>3</v>
-      </c>
-      <c r="B43" s="2">
-        <v>3</v>
-      </c>
-      <c r="C43" s="2">
-        <v>3</v>
-      </c>
-      <c r="D43" s="2">
-        <v>3</v>
-      </c>
-      <c r="E43" s="2">
-        <v>3</v>
-      </c>
-      <c r="F43" s="2">
+      <c r="A43" s="1">
+        <v>3</v>
+      </c>
+      <c r="B43" s="1">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1">
+        <v>3</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3</v>
+      </c>
+      <c r="F43" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>2.5</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>2.5</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <v>2.5</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="1">
         <v>2.5</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="1">
         <v>2.5</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="1">
         <v>2.5</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>5</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>2.5</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <v>2.5</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="1">
         <v>2.5</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="1">
         <v>2.5</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
+      <c r="A47" s="1">
         <v>5</v>
       </c>
-      <c r="B47" s="7">
-        <v>7</v>
-      </c>
-      <c r="C47" s="7">
-        <v>7</v>
-      </c>
-      <c r="D47" s="7">
-        <v>7</v>
-      </c>
-      <c r="E47" s="7">
-        <v>7</v>
-      </c>
-      <c r="F47" s="2">
+      <c r="B47" s="3">
+        <v>7</v>
+      </c>
+      <c r="C47" s="3">
+        <v>7</v>
+      </c>
+      <c r="D47" s="3">
+        <v>7</v>
+      </c>
+      <c r="E47" s="3">
+        <v>7</v>
+      </c>
+      <c r="F47" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>5</v>
       </c>
-      <c r="B48" s="7">
-        <v>7</v>
-      </c>
-      <c r="C48" s="7">
+      <c r="B48" s="3">
+        <v>7</v>
+      </c>
+      <c r="C48" s="3">
         <v>8.5</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="3">
         <v>8.5</v>
       </c>
-      <c r="E48" s="7">
-        <v>7</v>
-      </c>
-      <c r="F48" s="2">
+      <c r="E48" s="3">
+        <v>7</v>
+      </c>
+      <c r="F48" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>5</v>
       </c>
-      <c r="B49" s="7">
-        <v>7</v>
-      </c>
-      <c r="C49" s="7">
+      <c r="B49" s="3">
+        <v>7</v>
+      </c>
+      <c r="C49" s="3">
         <v>9.5</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="3">
         <v>9.5</v>
       </c>
-      <c r="E49" s="7">
-        <v>7</v>
-      </c>
-      <c r="F49" s="2">
+      <c r="E49" s="3">
+        <v>7</v>
+      </c>
+      <c r="F49" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>5</v>
       </c>
-      <c r="B50" s="7">
-        <v>7</v>
-      </c>
-      <c r="C50" s="7">
+      <c r="B50" s="3">
+        <v>7</v>
+      </c>
+      <c r="C50" s="3">
         <v>9.5</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D50" s="3">
         <v>9.5</v>
       </c>
-      <c r="E50" s="7">
-        <v>7</v>
-      </c>
-      <c r="F50" s="2">
+      <c r="E50" s="3">
+        <v>7</v>
+      </c>
+      <c r="F50" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>5</v>
       </c>
-      <c r="B51" s="7">
-        <v>7</v>
-      </c>
-      <c r="C51" s="7">
+      <c r="B51" s="3">
+        <v>7</v>
+      </c>
+      <c r="C51" s="3">
         <v>8.5</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="3">
         <v>8.5</v>
       </c>
-      <c r="E51" s="7">
-        <v>7</v>
-      </c>
-      <c r="F51" s="2">
+      <c r="E51" s="3">
+        <v>7</v>
+      </c>
+      <c r="F51" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>5</v>
       </c>
-      <c r="B52" s="7">
-        <v>7</v>
-      </c>
-      <c r="C52" s="7">
-        <v>7</v>
-      </c>
-      <c r="D52" s="7">
-        <v>7</v>
-      </c>
-      <c r="E52" s="7">
-        <v>7</v>
-      </c>
-      <c r="F52" s="2">
+      <c r="B52" s="3">
+        <v>7</v>
+      </c>
+      <c r="C52" s="3">
+        <v>7</v>
+      </c>
+      <c r="D52" s="3">
+        <v>7</v>
+      </c>
+      <c r="E52" s="3">
+        <v>7</v>
+      </c>
+      <c r="F52" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
+      <c r="A53" s="1">
         <v>5</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>2.5</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="1">
         <v>2.5</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="1">
         <v>2.5</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53" s="1">
         <v>2.5</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F53" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
+      <c r="A54" s="1">
         <v>2.5</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>2.5</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="1">
         <v>2.5</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="1">
         <v>2.5</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54" s="1">
         <v>2.5</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F54" s="1">
         <v>2.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added old plot_panel function, Multi1 dataset
</commit_message>
<xml_diff>
--- a/Dataset Key.xlsx
+++ b/Dataset Key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlima/Documents/GitHub/reconfigurable-solar-cells/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56617E91-D929-934F-9DB5-143C6B3F9805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6567C0-299C-9A46-92B3-F50FFD6EC871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-10060" windowWidth="38400" windowHeight="21100" xr2:uid="{D03FEAF9-A323-DD42-AAE4-45997B47A029}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{D03FEAF9-A323-DD42-AAE4-45997B47A029}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Shading Map Code</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Last column at 3, rest at 7</t>
   </si>
   <si>
-    <t>Second row at 3, rest at 7</t>
-  </si>
-  <si>
     <t>S03P5</t>
   </si>
   <si>
@@ -141,6 +138,26 @@
   </si>
   <si>
     <t>Improvement</t>
+  </si>
+  <si>
+    <t>First two rows at 3, rest at 7</t>
+  </si>
+  <si>
+    <t>Multi 1</t>
+  </si>
+  <si>
+    <t>﻿map1 = np.full((10, 6), 10)
+map1[:,:2] = 3
+map2 = np.copy(map1)
+map3 = np.copy(map1)
+map2[:,:4] = 3
+map3 = np.triu(np.full((10, 6), 10))</t>
+  </si>
+  <si>
+    <t>Low VMP = 0.7V</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
   </si>
 </sst>
 </file>
@@ -895,15 +912,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1016000</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>2478893</xdr:rowOff>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104969</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3893736</xdr:colOff>
+      <xdr:colOff>3810000</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1898023</xdr:rowOff>
+      <xdr:rowOff>1885322</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -926,8 +943,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7843520" y="28539293"/>
-          <a:ext cx="2877736" cy="1918490"/>
+          <a:off x="7962900" y="28832369"/>
+          <a:ext cx="2667000" cy="1780353"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1234,7 +1251,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9155723" y="16315592"/>
+          <a:off x="9156700" y="16319500"/>
           <a:ext cx="1771650" cy="1181100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1895,11 +1912,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5A1329-3D34-824E-9BD6-BFD7C34C5F99}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1915,7 +1932,7 @@
     <col min="12" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1929,28 +1946,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="210" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="210" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -1985,7 +2002,7 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="177" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -2019,8 +2036,11 @@
       <c r="K3" s="6">
         <v>125000</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="170" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="170" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -2053,7 +2073,7 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="146" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -2083,12 +2103,12 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="188" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="188" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="6" t="str">
-        <f t="shared" ref="B6:B18" si="1">_xlfn.CONCAT(A6,".xslx")</f>
+        <f t="shared" ref="B6:B19" si="1">_xlfn.CONCAT(A6,".xslx")</f>
         <v>S01P5.xslx</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2118,7 +2138,7 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="241" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="241" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -2127,7 +2147,7 @@
         <v>S02P5.xslx</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6">
@@ -2153,16 +2173,16 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="241" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="241" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>S03P5.xslx</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6">
@@ -2188,7 +2208,7 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="224" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="224" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
@@ -2221,9 +2241,9 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="223" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="223" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="6" t="str">
         <f t="shared" si="1"/>
@@ -2254,9 +2274,9 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="229" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="229" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="6" t="str">
         <f t="shared" si="1"/>
@@ -2287,9 +2307,9 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="197" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="197" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="6" t="str">
         <f t="shared" si="1"/>
@@ -2320,9 +2340,9 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="157" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="157" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="6" t="str">
         <f t="shared" si="1"/>
@@ -2337,7 +2357,7 @@
         <v>87.9</v>
       </c>
       <c r="G13" s="6">
-        <v>27.04</v>
+        <v>87.9</v>
       </c>
       <c r="H13" s="6">
         <v>192.71</v>
@@ -2353,9 +2373,9 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="196" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="196" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="6" t="str">
         <f t="shared" si="1"/>
@@ -2370,7 +2390,7 @@
         <v>87.9</v>
       </c>
       <c r="G14" s="6">
-        <v>27.04</v>
+        <v>87.9</v>
       </c>
       <c r="H14" s="6">
         <v>192.71</v>
@@ -2386,9 +2406,9 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="202" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="202" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="6" t="str">
         <f t="shared" si="1"/>
@@ -2419,9 +2439,9 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="224" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="224" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="6" t="str">
         <f t="shared" si="1"/>
@@ -2454,14 +2474,14 @@
     </row>
     <row r="17" spans="1:11" ht="169" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="6" t="str">
         <f t="shared" si="1"/>
         <v>T01P5.xslx</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6">
@@ -2489,14 +2509,14 @@
     </row>
     <row r="18" spans="1:11" ht="198" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6" t="str">
         <f t="shared" si="1"/>
         <v>T02P5.xslx</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6">
@@ -2521,6 +2541,105 @@
       <c r="K18" s="6">
         <v>64000</v>
       </c>
+    </row>
+    <row r="19" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Multi 1.xslx</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6">
+        <v>126.51</v>
+      </c>
+      <c r="G19" s="6">
+        <v>126.51</v>
+      </c>
+      <c r="H19" s="6">
+        <v>126.51</v>
+      </c>
+      <c r="I19" s="6">
+        <v>126.51</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6">
+        <v>119.11</v>
+      </c>
+      <c r="G20" s="6">
+        <v>119.11</v>
+      </c>
+      <c r="H20" s="6">
+        <v>119.11</v>
+      </c>
+      <c r="I20" s="6">
+        <v>119.11</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
+        <v>42.14</v>
+      </c>
+      <c r="I21" s="6">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="6">
+        <v>106</v>
+      </c>
+      <c r="F22" s="6">
+        <f>AVERAGE(F19:F21)</f>
+        <v>81.873333333333335</v>
+      </c>
+      <c r="G22" s="6">
+        <f>AVERAGE(G19:G21)</f>
+        <v>81.873333333333335</v>
+      </c>
+      <c r="H22" s="6">
+        <f>AVERAGE(H19:H21)</f>
+        <v>95.92</v>
+      </c>
+      <c r="I22" s="6">
+        <f>AVERAGE(I19:I21)</f>
+        <v>94.15333333333335</v>
+      </c>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:J1048576">
@@ -2537,8 +2656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC721700-1AB0-104E-99BB-9F6A073030E6}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2623,7 +2742,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>